<commit_message>
Add updated spreadsheet and new database table image
</commit_message>
<xml_diff>
--- a/p1-3_1-3 NF.xlsx
+++ b/p1-3_1-3 NF.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GoIT\DB\goit-rdb-hw-02\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E330960-B0C2-4A6C-B6FE-4199CF32D571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-20610" yWindow="2130" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Аркуш1" sheetId="1" r:id="rId4"/>
+    <sheet name="Аркуш1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -100,24 +109,26 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -128,11 +139,17 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -146,44 +163,40 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -373,35 +386,41 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="B2:O28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E16" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31:Q31"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="4.75"/>
-    <col customWidth="1" min="2" max="2" width="17.25"/>
-    <col customWidth="1" min="3" max="3" width="20.5"/>
-    <col customWidth="1" min="4" max="4" width="13.13"/>
-    <col customWidth="1" min="5" max="6" width="15.75"/>
-    <col customWidth="1" min="8" max="8" width="15.75"/>
-    <col customWidth="1" min="9" max="9" width="7.75"/>
-    <col customWidth="1" min="12" max="12" width="9.13"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="5" max="6" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2">
+    <row r="2" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" ht="18.0" customHeight="1">
+    <row r="3" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -418,9 +437,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B4" s="3">
-        <v>101.0</v>
+        <v>101</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
@@ -429,15 +448,15 @@
         <v>7</v>
       </c>
       <c r="E4" s="4">
-        <v>45000.0</v>
+        <v>45000</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B5" s="3">
-        <v>102.0</v>
+        <v>102</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>9</v>
@@ -446,15 +465,15 @@
         <v>10</v>
       </c>
       <c r="E5" s="4">
-        <v>45001.0</v>
+        <v>45001</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B6" s="3">
-        <v>103.0</v>
+        <v>103</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>12</v>
@@ -463,18 +482,18 @@
         <v>13</v>
       </c>
       <c r="E6" s="4">
-        <v>45002.0</v>
+        <v>45002</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B10" s="5" t="s">
         <v>1</v>
       </c>
@@ -494,92 +513,92 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B11" s="3">
-        <v>101.0</v>
+        <v>101</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="3">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F11" s="4">
-        <v>45000.0</v>
+        <v>45000</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B12" s="3">
-        <v>101.0</v>
+        <v>101</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D12" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F12" s="4">
-        <v>45000.0</v>
+        <v>45000</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B13" s="3">
-        <v>102.0</v>
+        <v>102</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D13" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F13" s="4">
-        <v>45001.0</v>
+        <v>45001</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B14" s="3">
-        <v>103.0</v>
+        <v>103</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F14" s="4">
-        <v>45002.0</v>
+        <v>45002</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
         <v>22</v>
       </c>
@@ -608,9 +627,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B18" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>8</v>
@@ -619,27 +638,27 @@
         <v>7</v>
       </c>
       <c r="F18" s="3">
-        <v>101.0</v>
+        <v>101</v>
       </c>
       <c r="G18" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H18" s="4">
-        <v>45000.0</v>
+        <v>45000</v>
       </c>
       <c r="J18" s="3">
-        <v>101.0</v>
+        <v>101</v>
       </c>
       <c r="K18" s="3" t="s">
         <v>18</v>
       </c>
       <c r="L18" s="3">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B19" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>11</v>
@@ -648,27 +667,27 @@
         <v>10</v>
       </c>
       <c r="F19" s="3">
-        <v>102.0</v>
+        <v>102</v>
       </c>
       <c r="G19" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="H19" s="4">
-        <v>45001.0</v>
+        <v>45001</v>
       </c>
       <c r="J19" s="3">
-        <v>101.0</v>
+        <v>101</v>
       </c>
       <c r="K19" s="3" t="s">
         <v>19</v>
       </c>
       <c r="L19" s="3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B20" s="3">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>14</v>
@@ -677,41 +696,41 @@
         <v>13</v>
       </c>
       <c r="F20" s="3">
-        <v>103.0</v>
+        <v>103</v>
       </c>
       <c r="G20" s="3">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="H20" s="4">
-        <v>45002.0</v>
+        <v>45002</v>
       </c>
       <c r="J20" s="3">
-        <v>102.0</v>
+        <v>102</v>
       </c>
       <c r="K20" s="3" t="s">
         <v>20</v>
       </c>
       <c r="L20" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J21" s="3">
-        <v>103.0</v>
+        <v>103</v>
       </c>
       <c r="K21" s="3" t="s">
         <v>19</v>
       </c>
       <c r="L21" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B24" s="5" t="s">
         <v>22</v>
       </c>
@@ -746,9 +765,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B25" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>8</v>
@@ -757,33 +776,33 @@
         <v>7</v>
       </c>
       <c r="F25" s="3">
-        <v>101.0</v>
+        <v>101</v>
       </c>
       <c r="G25" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H25" s="4">
-        <v>45000.0</v>
+        <v>45000</v>
       </c>
       <c r="J25" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K25" s="3" t="s">
         <v>18</v>
       </c>
       <c r="M25" s="3">
-        <v>101.0</v>
+        <v>101</v>
       </c>
       <c r="N25" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="O25" s="3">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B26" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>11</v>
@@ -792,33 +811,33 @@
         <v>10</v>
       </c>
       <c r="F26" s="3">
-        <v>102.0</v>
+        <v>102</v>
       </c>
       <c r="G26" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="H26" s="4">
-        <v>45001.0</v>
+        <v>45001</v>
       </c>
       <c r="J26" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="K26" s="3" t="s">
         <v>19</v>
       </c>
       <c r="M26" s="3">
-        <v>101.0</v>
+        <v>101</v>
       </c>
       <c r="N26" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="O26" s="3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B27" s="3">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>14</v>
@@ -827,42 +846,42 @@
         <v>13</v>
       </c>
       <c r="F27" s="3">
-        <v>103.0</v>
+        <v>103</v>
       </c>
       <c r="G27" s="3">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="H27" s="4">
-        <v>45002.0</v>
+        <v>45002</v>
       </c>
       <c r="J27" s="3">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="K27" s="3" t="s">
         <v>20</v>
       </c>
       <c r="M27" s="3">
-        <v>102.0</v>
+        <v>102</v>
       </c>
       <c r="N27" s="3">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="O27" s="3">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="M28" s="3">
-        <v>103.0</v>
+        <v>103</v>
       </c>
       <c r="N28" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="O28" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>